<commit_message>
js files are added in foorter and one graph is at dashboard
</commit_message>
<xml_diff>
--- a/uploads/attachments/2020/FebMobile subs.xlsx
+++ b/uploads/attachments/2020/FebMobile subs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bhutan Code Challenge-2019\BHUTAN STARTUP HACKATHON CHALLENGE\after event\data\subs\Mobile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\Super Final data\subs\Mobile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7605" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7605" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="JAN" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:J34"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +550,7 @@
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -5424,8 +5424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:J34"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6646,8 +6646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection sqref="A1:J33"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7869,7 +7869,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:J34"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9090,8 +9090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J33"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10310,8 +10310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>